<commit_message>
Adding parameters from TestNG file
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richari\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D11BE392-D5DA-4F9E-A418-B826F685E8F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{1C0C6ECF-35EA-4A51-81CD-797F25BD4435}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
     <sheet name="Deals" sheetId="2" r:id="rId2"/>
     <sheet name="Tasks" sheetId="3" r:id="rId3"/>
+    <sheet name="Events" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Title</t>
   </si>
@@ -81,12 +76,36 @@
   </si>
   <si>
     <t>Google</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>10:00AM</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Message</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,6 +125,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -137,10 +162,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -201,7 +232,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -253,7 +284,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -447,17 +478,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0E0FC7-D7D5-41CD-A18E-78FCA34DD78C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
@@ -530,7 +561,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F87E34-42DC-42CA-AD7D-1A1E307C4C45}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -542,7 +573,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090766E8-4524-48FE-B0E4-477DE73F6A57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -551,4 +582,59 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="5"/>
+    <col min="3" max="3" width="12.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>